<commit_message>
finished 9-10 and just need to do 11!
</commit_message>
<xml_diff>
--- a/Lab 10/4YearResults.xlsx
+++ b/Lab 10/4YearResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14320" yWindow="0" windowWidth="14460" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="2240" yWindow="0" windowWidth="26540" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,12 +73,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -108,6 +112,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,12 +130,49 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -131,10 +181,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -471,172 +531,182 @@
   <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="C3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>0.74916839999999996</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>0.56137144999999999</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>0.11380832</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>0.23593839999999999</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>9.3723103000000005</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>5.1514782600000002</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="7">
         <v>5.6970002800000001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>5.1992532000000002</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" t="s">
+      <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>4.4484579999999996</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>5.7904184499999998</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="7">
         <v>4.2627603699999996</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>5.0333231999999999</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" t="s">
+      <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>0.15723000000000001</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>0.18349713000000001</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="7">
         <v>0.10304143</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>0.1240797</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" t="s">
+      <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>74.8874706</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>71.675066200000003</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="7">
         <v>66.521281459999997</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>7.3505694999999998</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" t="s">
+      <c r="B9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>1.6897789000000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>1.24295723</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="7">
         <v>1.0167135599999999</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>3.9484645999999999</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" t="s">
+      <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>5.7509900000000003E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>5.5464439999999997E-2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="7">
         <v>5.2303339999999997E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>0.101164</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="8">
         <v>0.44843175000000002</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <v>0.66781080999999998</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="9">
         <v>0.64347839338000001</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="8">
         <v>0.63252699999999995</v>
       </c>
     </row>

</xml_diff>